<commit_message>
preparation release 405 24f4ac48e92c6fc0d65f62aa18aff309d16dd3ec
</commit_message>
<xml_diff>
--- a/341-préparation-release-405/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/341-préparation-release-405/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.4</t>
+    <t>4.0.5</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-09T09:24:12+00:00</t>
+    <t>2025-10-09T09:53:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>